<commit_message>
Moved file args out of calling command, sends mail now
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Client's First Name</t>
+  </si>
+  <si>
+    <t>Client's Last Name</t>
+  </si>
+  <si>
+    <t>Clinet's Email Address</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>tsevans@vt.edu</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +51,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,14 +88,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -144,6 +208,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +260,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -331,12 +429,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="17.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working with excel file reads
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Client's First Name</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>tsevans@vt.edu</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Boland</t>
+  </si>
+  <si>
+    <t>cboland@utexas.edu</t>
   </si>
 </sst>
 </file>
@@ -109,10 +118,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -429,19 +441,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+    <col min="1" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +464,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -461,6 +473,17 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>